<commit_message>
Updated excel till end of the 06.11.2024
Updated excel till end of the 06.11.2024
</commit_message>
<xml_diff>
--- a/Bytexl guided projects-Oct 28-Oct 30-tracking sheet for educators - new.xlsx
+++ b/Bytexl guided projects-Oct 28-Oct 30-tracking sheet for educators - new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Parul - NET\Project Guided Support - Documents\Final Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83D3DC3-31CE-4F2E-8959-E93CCDE3C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09BE7A8-8313-46AB-BA1E-20B9B5F4F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE489B8A-5E2C-4E4C-86C0-98B32BDB1FB5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>Activity</t>
   </si>
@@ -461,6 +461,93 @@
   </si>
   <si>
     <t xml:space="preserve">Push commit work on GitHub ( Backend commit - 4 ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push commit work on GitHub ( Backend commit - 5 ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push commit work on GitHub ( Backend commit - 6 ) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Model class ( ServiceCenterMaster), Repository, Service, and Controller and test it in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>postman</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to ensure end point and data operation is working as expected</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Model class ( VehiclerMaster), Repository, Service, and Controller and test it in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>postman</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to ensure end point and data operation is working as expected</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Model class ( VehicleServiceMaster), Repository, Service, and Controller and test it in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>postman</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to ensure end point and data operation is working as expected</t>
+    </r>
+  </si>
+  <si>
+    <t>Completed the ServiceCenterMaster, VehicleMaster and VehicleServiceEntry CRUD operation and check in postman as well to ensure endpoint is working fine</t>
   </si>
 </sst>
 </file>
@@ -599,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -682,14 +769,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1231,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A149F8-039D-421A-AE07-08EEFD0B1E24}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1296,7 +1389,7 @@
     <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
       <c r="B3" s="26"/>
-      <c r="C3" s="31"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="18" t="s">
         <v>43</v>
       </c>
@@ -1309,7 +1402,7 @@
     <row r="4" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="26"/>
-      <c r="C4" s="31"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="12" t="s">
         <v>62</v>
       </c>
@@ -1322,7 +1415,7 @@
     <row r="5" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="31"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="12" t="s">
         <v>61</v>
       </c>
@@ -1335,7 +1428,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="18" t="s">
         <v>45</v>
       </c>
@@ -1352,7 +1445,7 @@
       <c r="B7" s="26">
         <v>45599</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="12" t="s">
         <v>60</v>
       </c>
@@ -1369,7 +1462,7 @@
     <row r="8" spans="1:7" ht="54" x14ac:dyDescent="0.3">
       <c r="A8" s="25"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="12" t="s">
         <v>59</v>
       </c>
@@ -1382,7 +1475,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="18" t="s">
         <v>50</v>
       </c>
@@ -1399,7 +1492,7 @@
       <c r="B10" s="26">
         <v>45600</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
@@ -1416,7 +1509,7 @@
     <row r="11" spans="1:7" ht="54" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="26"/>
-      <c r="C11" s="31"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="12" t="s">
         <v>57</v>
       </c>
@@ -1429,7 +1522,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="18" t="s">
         <v>51</v>
       </c>
@@ -1446,7 +1539,7 @@
       <c r="B13" s="26">
         <v>45601</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="12" t="s">
         <v>55</v>
       </c>
@@ -1463,7 +1556,7 @@
     <row r="14" spans="1:7" ht="54" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
       <c r="B14" s="26"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1476,7 +1569,7 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="26"/>
-      <c r="C15" s="32"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="18" t="s">
         <v>63</v>
       </c>
@@ -1486,13 +1579,91 @@
       <c r="F15" s="27"/>
       <c r="G15" s="29"/>
     </row>
+    <row r="16" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>4</v>
+      </c>
+      <c r="B16" s="26">
+        <v>45601</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+    </row>
+    <row r="19" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="C2:C20"/>
+    <mergeCell ref="F16:F20"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="G13:G15"/>
-    <mergeCell ref="C2:C15"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="F10:F12"/>
@@ -1504,7 +1675,6 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="G2:G6"/>
-    <mergeCell ref="F2:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{7C388FCA-351F-407B-9AEF-2C581D300F3F}"/>

</xml_diff>